<commit_message>
MO, MSFT, Screener Update
</commit_message>
<xml_diff>
--- a/MO.xlsx
+++ b/MO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28AB469-CCE3-469D-88EC-1F05A20DBFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738113E5-F816-4A1A-B483-24811E92445A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3135" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Price</t>
   </si>
@@ -203,19 +211,64 @@
   </si>
   <si>
     <t>Oral Tobacco Y/Y</t>
+  </si>
+  <si>
+    <t>Net Earnings Y/Y</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Terminal</t>
+  </si>
+  <si>
+    <t>NPV</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>underperformed spy for the last 10 years</t>
+  </si>
+  <si>
+    <t>Phillip Morris (PM)</t>
+  </si>
+  <si>
+    <t>British Tobacco (BTI)</t>
+  </si>
+  <si>
+    <t>cant invest in e-cigarretes</t>
+  </si>
+  <si>
+    <t>chewing tobacco best in the industry 42% market share</t>
+  </si>
+  <si>
+    <t>Competitors:</t>
+  </si>
+  <si>
+    <t>dividend rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -260,7 +313,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -268,27 +321,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="38" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -312,7 +446,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
+      <xdr:colOff>607695</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
@@ -335,8 +469,58 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10713720" y="15240"/>
-          <a:ext cx="15240" cy="6507480"/>
+          <a:off x="10447020" y="15240"/>
+          <a:ext cx="9525" cy="7423785"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8412C5D0-71D6-8166-1D8E-99A349F98E95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="25069800" y="19050"/>
+          <a:ext cx="9525" cy="6134100"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -625,20 +809,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="L2:M7"/>
+  <dimension ref="C2:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="9.109375" style="1"/>
+    <col min="1" max="11" width="9.140625" style="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
       <c r="L2" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,7 +830,10 @@
         <v>44.22</v>
       </c>
     </row>
-    <row r="3" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C3" s="16" t="s">
+        <v>64</v>
+      </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
       </c>
@@ -654,7 +841,10 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="4" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C4" s="16" t="s">
+        <v>67</v>
+      </c>
       <c r="L4" s="1" t="s">
         <v>2</v>
       </c>
@@ -663,7 +853,10 @@
         <v>79596</v>
       </c>
     </row>
-    <row r="5" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C5" s="16" t="s">
+        <v>68</v>
+      </c>
       <c r="L5" s="1" t="s">
         <v>3</v>
       </c>
@@ -671,7 +864,7 @@
         <v>2567</v>
       </c>
     </row>
-    <row r="6" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
@@ -679,7 +872,7 @@
         <v>2634</v>
       </c>
     </row>
-    <row r="7" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="L7" s="1" t="s">
         <v>5</v>
       </c>
@@ -687,6 +880,32 @@
         <f>M4-M5+M6</f>
         <v>79663</v>
       </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="28"/>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C14" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="29"/>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C15" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="29"/>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C16" s="30"/>
+      <c r="D16" s="29"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -696,29 +915,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3628CCE6-9C82-4B7C-8973-62026B03EF08}">
-  <dimension ref="A1:AL42"/>
+  <dimension ref="A1:DF42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AR30" sqref="AR30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.109375" style="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.109375" style="1"/>
-    <col min="10" max="10" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.109375" style="1"/>
-    <col min="14" max="14" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -765,7 +984,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:110" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
@@ -823,55 +1042,336 @@
       <c r="U2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="1">
         <v>2010</v>
       </c>
-      <c r="AB2" s="1">
-        <f>AA2+1</f>
+      <c r="AD2" s="1">
+        <f>AC2+1</f>
         <v>2011</v>
       </c>
-      <c r="AC2" s="1">
-        <f t="shared" ref="AC2:AO2" si="0">AB2+1</f>
+      <c r="AE2" s="1">
+        <f t="shared" ref="AE2:AN2" si="0">AD2+1</f>
         <v>2012</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AF2" s="1">
         <f t="shared" si="0"/>
         <v>2013</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AG2" s="1">
         <f t="shared" si="0"/>
         <v>2014</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AH2" s="1">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AI2" s="1">
         <f t="shared" si="0"/>
         <v>2016</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AJ2" s="1">
         <f t="shared" si="0"/>
         <v>2017</v>
       </c>
-      <c r="AI2" s="1">
+      <c r="AK2" s="1">
         <f t="shared" si="0"/>
         <v>2018</v>
       </c>
-      <c r="AJ2" s="1">
+      <c r="AL2" s="1">
         <f t="shared" si="0"/>
         <v>2019</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AM2" s="1">
         <f t="shared" si="0"/>
         <v>2020</v>
       </c>
-      <c r="AL2" s="1">
+      <c r="AN2" s="1">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AO2" s="1">
+        <f t="shared" ref="AO2" si="1">AN2+1</f>
+        <v>2022</v>
+      </c>
+      <c r="AP2" s="1">
+        <f t="shared" ref="AP2" si="2">AO2+1</f>
+        <v>2023</v>
+      </c>
+      <c r="AQ2" s="1">
+        <f t="shared" ref="AQ2" si="3">AP2+1</f>
+        <v>2024</v>
+      </c>
+      <c r="AR2" s="1">
+        <f t="shared" ref="AR2" si="4">AQ2+1</f>
+        <v>2025</v>
+      </c>
+      <c r="AS2" s="1">
+        <f t="shared" ref="AS2" si="5">AR2+1</f>
+        <v>2026</v>
+      </c>
+      <c r="AT2" s="1">
+        <f t="shared" ref="AT2" si="6">AS2+1</f>
+        <v>2027</v>
+      </c>
+      <c r="AU2" s="1">
+        <f t="shared" ref="AU2" si="7">AT2+1</f>
+        <v>2028</v>
+      </c>
+      <c r="AV2" s="1">
+        <f t="shared" ref="AV2" si="8">AU2+1</f>
+        <v>2029</v>
+      </c>
+      <c r="AW2" s="1">
+        <f t="shared" ref="AW2" si="9">AV2+1</f>
+        <v>2030</v>
+      </c>
+      <c r="AX2" s="1">
+        <f t="shared" ref="AX2" si="10">AW2+1</f>
+        <v>2031</v>
+      </c>
+      <c r="AY2" s="1">
+        <f t="shared" ref="AY2" si="11">AX2+1</f>
+        <v>2032</v>
+      </c>
+      <c r="AZ2" s="1">
+        <f t="shared" ref="AZ2" si="12">AY2+1</f>
+        <v>2033</v>
+      </c>
+      <c r="BA2" s="1">
+        <f t="shared" ref="BA2" si="13">AZ2+1</f>
+        <v>2034</v>
+      </c>
+      <c r="BB2" s="1">
+        <f t="shared" ref="BB2" si="14">BA2+1</f>
+        <v>2035</v>
+      </c>
+      <c r="BC2" s="1">
+        <f t="shared" ref="BC2" si="15">BB2+1</f>
+        <v>2036</v>
+      </c>
+      <c r="BD2" s="1">
+        <f t="shared" ref="BD2" si="16">BC2+1</f>
+        <v>2037</v>
+      </c>
+      <c r="BE2" s="1">
+        <f t="shared" ref="BE2" si="17">BD2+1</f>
+        <v>2038</v>
+      </c>
+      <c r="BF2" s="1">
+        <f t="shared" ref="BF2" si="18">BE2+1</f>
+        <v>2039</v>
+      </c>
+      <c r="BG2" s="1">
+        <f t="shared" ref="BG2" si="19">BF2+1</f>
+        <v>2040</v>
+      </c>
+      <c r="BH2" s="1">
+        <f t="shared" ref="BH2" si="20">BG2+1</f>
+        <v>2041</v>
+      </c>
+      <c r="BI2" s="1">
+        <f t="shared" ref="BI2" si="21">BH2+1</f>
+        <v>2042</v>
+      </c>
+      <c r="BJ2" s="1">
+        <f t="shared" ref="BJ2" si="22">BI2+1</f>
+        <v>2043</v>
+      </c>
+      <c r="BK2" s="1">
+        <f t="shared" ref="BK2" si="23">BJ2+1</f>
+        <v>2044</v>
+      </c>
+      <c r="BL2" s="1">
+        <f t="shared" ref="BL2" si="24">BK2+1</f>
+        <v>2045</v>
+      </c>
+      <c r="BM2" s="1">
+        <f t="shared" ref="BM2" si="25">BL2+1</f>
+        <v>2046</v>
+      </c>
+      <c r="BN2" s="1">
+        <f t="shared" ref="BN2" si="26">BM2+1</f>
+        <v>2047</v>
+      </c>
+      <c r="BO2" s="1">
+        <f t="shared" ref="BO2" si="27">BN2+1</f>
+        <v>2048</v>
+      </c>
+      <c r="BP2" s="1">
+        <f t="shared" ref="BP2" si="28">BO2+1</f>
+        <v>2049</v>
+      </c>
+      <c r="BQ2" s="1">
+        <f t="shared" ref="BQ2" si="29">BP2+1</f>
+        <v>2050</v>
+      </c>
+      <c r="BR2" s="1">
+        <f t="shared" ref="BR2" si="30">BQ2+1</f>
+        <v>2051</v>
+      </c>
+      <c r="BS2" s="1">
+        <f t="shared" ref="BS2" si="31">BR2+1</f>
+        <v>2052</v>
+      </c>
+      <c r="BT2" s="1">
+        <f t="shared" ref="BT2" si="32">BS2+1</f>
+        <v>2053</v>
+      </c>
+      <c r="BU2" s="1">
+        <f t="shared" ref="BU2" si="33">BT2+1</f>
+        <v>2054</v>
+      </c>
+      <c r="BV2" s="1">
+        <f t="shared" ref="BV2" si="34">BU2+1</f>
+        <v>2055</v>
+      </c>
+      <c r="BW2" s="1">
+        <f t="shared" ref="BW2" si="35">BV2+1</f>
+        <v>2056</v>
+      </c>
+      <c r="BX2" s="1">
+        <f t="shared" ref="BX2" si="36">BW2+1</f>
+        <v>2057</v>
+      </c>
+      <c r="BY2" s="1">
+        <f t="shared" ref="BY2" si="37">BX2+1</f>
+        <v>2058</v>
+      </c>
+      <c r="BZ2" s="1">
+        <f t="shared" ref="BZ2" si="38">BY2+1</f>
+        <v>2059</v>
+      </c>
+      <c r="CA2" s="1">
+        <f t="shared" ref="CA2" si="39">BZ2+1</f>
+        <v>2060</v>
+      </c>
+      <c r="CB2" s="1">
+        <f t="shared" ref="CB2" si="40">CA2+1</f>
+        <v>2061</v>
+      </c>
+      <c r="CC2" s="1">
+        <f t="shared" ref="CC2" si="41">CB2+1</f>
+        <v>2062</v>
+      </c>
+      <c r="CD2" s="1">
+        <f t="shared" ref="CD2" si="42">CC2+1</f>
+        <v>2063</v>
+      </c>
+      <c r="CE2" s="1">
+        <f t="shared" ref="CE2" si="43">CD2+1</f>
+        <v>2064</v>
+      </c>
+      <c r="CF2" s="1">
+        <f t="shared" ref="CF2" si="44">CE2+1</f>
+        <v>2065</v>
+      </c>
+      <c r="CG2" s="1">
+        <f t="shared" ref="CG2" si="45">CF2+1</f>
+        <v>2066</v>
+      </c>
+      <c r="CH2" s="1">
+        <f t="shared" ref="CH2" si="46">CG2+1</f>
+        <v>2067</v>
+      </c>
+      <c r="CI2" s="1">
+        <f t="shared" ref="CI2" si="47">CH2+1</f>
+        <v>2068</v>
+      </c>
+      <c r="CJ2" s="1">
+        <f t="shared" ref="CJ2" si="48">CI2+1</f>
+        <v>2069</v>
+      </c>
+      <c r="CK2" s="1">
+        <f t="shared" ref="CK2" si="49">CJ2+1</f>
+        <v>2070</v>
+      </c>
+      <c r="CL2" s="1">
+        <f t="shared" ref="CL2" si="50">CK2+1</f>
+        <v>2071</v>
+      </c>
+      <c r="CM2" s="1">
+        <f t="shared" ref="CM2" si="51">CL2+1</f>
+        <v>2072</v>
+      </c>
+      <c r="CN2" s="1">
+        <f t="shared" ref="CN2" si="52">CM2+1</f>
+        <v>2073</v>
+      </c>
+      <c r="CO2" s="1">
+        <f t="shared" ref="CO2" si="53">CN2+1</f>
+        <v>2074</v>
+      </c>
+      <c r="CP2" s="1">
+        <f t="shared" ref="CP2" si="54">CO2+1</f>
+        <v>2075</v>
+      </c>
+      <c r="CQ2" s="1">
+        <f t="shared" ref="CQ2" si="55">CP2+1</f>
+        <v>2076</v>
+      </c>
+      <c r="CR2" s="1">
+        <f t="shared" ref="CR2" si="56">CQ2+1</f>
+        <v>2077</v>
+      </c>
+      <c r="CS2" s="1">
+        <f t="shared" ref="CS2" si="57">CR2+1</f>
+        <v>2078</v>
+      </c>
+      <c r="CT2" s="1">
+        <f t="shared" ref="CT2" si="58">CS2+1</f>
+        <v>2079</v>
+      </c>
+      <c r="CU2" s="1">
+        <f t="shared" ref="CU2" si="59">CT2+1</f>
+        <v>2080</v>
+      </c>
+      <c r="CV2" s="1">
+        <f t="shared" ref="CV2" si="60">CU2+1</f>
+        <v>2081</v>
+      </c>
+      <c r="CW2" s="1">
+        <f t="shared" ref="CW2" si="61">CV2+1</f>
+        <v>2082</v>
+      </c>
+      <c r="CX2" s="1">
+        <f t="shared" ref="CX2" si="62">CW2+1</f>
+        <v>2083</v>
+      </c>
+      <c r="CY2" s="1">
+        <f t="shared" ref="CY2" si="63">CX2+1</f>
+        <v>2084</v>
+      </c>
+      <c r="CZ2" s="1">
+        <f t="shared" ref="CZ2" si="64">CY2+1</f>
+        <v>2085</v>
+      </c>
+      <c r="DA2" s="1">
+        <f t="shared" ref="DA2" si="65">CZ2+1</f>
+        <v>2086</v>
+      </c>
+      <c r="DB2" s="1">
+        <f t="shared" ref="DB2" si="66">DA2+1</f>
+        <v>2087</v>
+      </c>
+      <c r="DC2" s="1">
+        <f t="shared" ref="DC2" si="67">DB2+1</f>
+        <v>2088</v>
+      </c>
+      <c r="DD2" s="1">
+        <f t="shared" ref="DD2" si="68">DC2+1</f>
+        <v>2089</v>
+      </c>
+      <c r="DE2" s="1">
+        <f t="shared" ref="DE2" si="69">DD2+1</f>
+        <v>2090</v>
+      </c>
+      <c r="DF2" s="1">
+        <f t="shared" ref="DF2" si="70">DE2+1</f>
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="3" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
@@ -922,23 +1422,59 @@
         <v>6049.1900000000005</v>
       </c>
       <c r="R3" s="2">
-        <f t="shared" ref="R3:U3" si="1">Q3*1.03</f>
+        <f t="shared" ref="R3:U3" si="71">Q3*1.03</f>
         <v>6230.6657000000005</v>
       </c>
       <c r="S3" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="71"/>
         <v>6417.5856710000007</v>
       </c>
       <c r="T3" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="71"/>
         <v>6610.1132411300014</v>
       </c>
       <c r="U3" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="71"/>
         <v>6808.4166383639013</v>
       </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AC3" s="1">
+        <v>22191</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>21970</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>22216</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>21868</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>21939</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>22792</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>22851</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>22636</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>22297</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>21996</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>23089</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>22866</v>
+      </c>
+    </row>
+    <row r="4" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
@@ -989,23 +1525,59 @@
         <v>678.30000000000007</v>
       </c>
       <c r="R4" s="2">
-        <f t="shared" ref="R4:U4" si="2">Q4*1.02</f>
+        <f t="shared" ref="R4:U4" si="72">Q4*1.02</f>
         <v>691.8660000000001</v>
       </c>
       <c r="S4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="72"/>
         <v>705.70332000000008</v>
       </c>
       <c r="T4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="72"/>
         <v>719.81738640000015</v>
       </c>
       <c r="U4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="72"/>
         <v>734.21373412800017</v>
       </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AC4" s="1">
+        <v>1552</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>1627</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>1691</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>1778</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>1809</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>1879</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>2051</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>2155</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>2262</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>2367</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>2533</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>2608</v>
+      </c>
+    </row>
+    <row r="5" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1066,8 +1638,44 @@
       <c r="U5" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AC5" s="1">
+        <v>459</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>516</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>561</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>609</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>643</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>692</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>746</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>698</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>691</v>
+      </c>
+      <c r="AL5" s="1">
+        <v>689</v>
+      </c>
+      <c r="AM5" s="1">
+        <v>614</v>
+      </c>
+      <c r="AN5" s="1">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1121,56 +1729,92 @@
         <v>3.1500000000000004</v>
       </c>
       <c r="S6" s="14">
-        <f t="shared" ref="S6:U6" si="3">R6*1.05</f>
+        <f t="shared" ref="S6:U6" si="73">R6*1.05</f>
         <v>3.3075000000000006</v>
       </c>
       <c r="T6" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="73"/>
         <v>3.4728750000000006</v>
       </c>
       <c r="U6" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="73"/>
         <v>3.6465187500000007</v>
       </c>
-    </row>
-    <row r="7" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC6" s="1">
+        <v>161</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>-313</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>150</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>211</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>131</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>71</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>96</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>87</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>114</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>58</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>-83</v>
+      </c>
+      <c r="AN6" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:110" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" ref="C7:K7" si="4">SUM(C3:C6)</f>
+        <f t="shared" ref="C7:K7" si="74">SUM(C3:C6)</f>
         <v>5628</v>
       </c>
       <c r="D7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="74"/>
         <v>6619</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="74"/>
         <v>6856</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="74"/>
         <v>6007</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="74"/>
         <v>6359</v>
       </c>
       <c r="H7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="74"/>
         <v>6367</v>
       </c>
       <c r="I7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="74"/>
         <v>7123</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="74"/>
         <v>6304</v>
       </c>
       <c r="K7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="74"/>
         <v>6036</v>
       </c>
       <c r="L7" s="5">
@@ -1178,19 +1822,19 @@
         <v>6936</v>
       </c>
       <c r="M7" s="5">
-        <f t="shared" ref="M7:P7" si="5">SUM(M3:M6)</f>
+        <f t="shared" ref="M7:P7" si="75">SUM(M3:M6)</f>
         <v>6786</v>
       </c>
       <c r="N7" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="75"/>
         <v>6255</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="75"/>
         <v>5892</v>
       </c>
       <c r="P7" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="75"/>
         <v>6543</v>
       </c>
       <c r="Q7" s="2">
@@ -1198,23 +1842,74 @@
         <v>6730.4900000000007</v>
       </c>
       <c r="R7" s="2">
-        <f t="shared" ref="R7:U7" si="6">SUM(R3:R6)</f>
+        <f t="shared" ref="R7:U7" si="76">SUM(R3:R6)</f>
         <v>6925.6817000000001</v>
       </c>
       <c r="S7" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="76"/>
         <v>7126.5964910000012</v>
       </c>
       <c r="T7" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="76"/>
         <v>7333.4035025300018</v>
       </c>
       <c r="U7" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="76"/>
         <v>7546.2768912419015</v>
       </c>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5">
+        <f t="shared" ref="Z7:AL7" si="77">SUM(AC3:AC6)</f>
+        <v>24363</v>
+      </c>
+      <c r="AD7" s="5">
+        <f t="shared" si="77"/>
+        <v>23800</v>
+      </c>
+      <c r="AE7" s="5">
+        <f t="shared" si="77"/>
+        <v>24618</v>
+      </c>
+      <c r="AF7" s="5">
+        <f t="shared" si="77"/>
+        <v>24466</v>
+      </c>
+      <c r="AG7" s="5">
+        <f t="shared" si="77"/>
+        <v>24522</v>
+      </c>
+      <c r="AH7" s="5">
+        <f t="shared" si="77"/>
+        <v>25434</v>
+      </c>
+      <c r="AI7" s="5">
+        <f t="shared" si="77"/>
+        <v>25744</v>
+      </c>
+      <c r="AJ7" s="5">
+        <f t="shared" si="77"/>
+        <v>25576</v>
+      </c>
+      <c r="AK7" s="5">
+        <f t="shared" si="77"/>
+        <v>25364</v>
+      </c>
+      <c r="AL7" s="5">
+        <f t="shared" ref="AL7:AN7" si="78">SUM(AL3:AL6)</f>
+        <v>25110</v>
+      </c>
+      <c r="AM7" s="5">
+        <f t="shared" si="78"/>
+        <v>26153</v>
+      </c>
+      <c r="AN7" s="5">
+        <f t="shared" si="78"/>
+        <v>26013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1265,23 +1960,59 @@
         <v>1749.9274000000003</v>
       </c>
       <c r="R8" s="2">
-        <f t="shared" ref="R8:U8" si="7">R7*0.26</f>
+        <f t="shared" ref="R8:U8" si="79">R7*0.26</f>
         <v>1800.677242</v>
       </c>
       <c r="S8" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="79"/>
         <v>1852.9150876600004</v>
       </c>
       <c r="T8" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="79"/>
         <v>1906.6849106578006</v>
       </c>
       <c r="U8" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="79"/>
         <v>1962.0319917228944</v>
       </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AC8" s="1">
+        <v>7704</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>7680</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>7937</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>7206</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>7785</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>7740</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>7765</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>7531</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>7373</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>7085</v>
+      </c>
+      <c r="AM8" s="1">
+        <v>7818</v>
+      </c>
+      <c r="AN8" s="1">
+        <v>7119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1332,23 +2063,59 @@
         <v>1346.0980000000002</v>
       </c>
       <c r="R9" s="2">
-        <f t="shared" ref="R9:U9" si="8">R7*0.2</f>
+        <f t="shared" ref="R9:U9" si="80">R7*0.2</f>
         <v>1385.13634</v>
       </c>
       <c r="S9" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="80"/>
         <v>1425.3192982000003</v>
       </c>
       <c r="T9" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="80"/>
         <v>1466.6807005060004</v>
       </c>
       <c r="U9" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="80"/>
         <v>1509.2553782483803</v>
       </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AC9" s="1">
+        <v>7471</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>7181</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>7118</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>6803</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>6577</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>6580</v>
+      </c>
+      <c r="AI9" s="1">
+        <v>6407</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>6082</v>
+      </c>
+      <c r="AK9" s="1">
+        <v>5737</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>5314</v>
+      </c>
+      <c r="AM9" s="1">
+        <v>5312</v>
+      </c>
+      <c r="AN9" s="1">
+        <v>4902</v>
+      </c>
+    </row>
+    <row r="10" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1399,23 +2166,59 @@
         <v>3028.7205000000004</v>
       </c>
       <c r="R10" s="2">
-        <f t="shared" ref="R10:U10" si="9">R7-(R11+R8+R9)</f>
+        <f t="shared" ref="R10:U10" si="81">R7-(R11+R8+R9)</f>
         <v>3116.5567650000003</v>
       </c>
       <c r="S10" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="81"/>
         <v>3206.9684209500001</v>
       </c>
       <c r="T10" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="81"/>
         <v>3300.0315761385004</v>
       </c>
       <c r="U10" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="81"/>
         <v>3395.8246010588555</v>
       </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AC10" s="1">
+        <v>9188</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>8939</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>9563</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>10457</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>10160</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>11114</v>
+      </c>
+      <c r="AI10" s="1">
+        <v>11572</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>11963</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>12254</v>
+      </c>
+      <c r="AL10" s="1">
+        <v>12711</v>
+      </c>
+      <c r="AM10" s="1">
+        <v>13023</v>
+      </c>
+      <c r="AN10" s="1">
+        <v>13992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1466,32 +2269,68 @@
         <v>605.7441</v>
       </c>
       <c r="R11" s="2">
-        <f t="shared" ref="R11:U11" si="10">R7*0.09</f>
+        <f t="shared" ref="R11:U11" si="82">R7*0.09</f>
         <v>623.31135299999994</v>
       </c>
       <c r="S11" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="82"/>
         <v>641.39368419000004</v>
       </c>
       <c r="T11" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="82"/>
         <v>660.00631522770016</v>
       </c>
       <c r="U11" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="82"/>
         <v>679.16492021177112</v>
       </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AC11" s="1">
+        <v>2735</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>2643</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>2281</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>2340</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>2539</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>2708</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>2662</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>2338</v>
+      </c>
+      <c r="AK11" s="1">
+        <v>2756</v>
+      </c>
+      <c r="AL11" s="1">
+        <v>2226</v>
+      </c>
+      <c r="AM11" s="1">
+        <v>2154</v>
+      </c>
+      <c r="AN11" s="1">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="12" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" ref="C12:K12" si="11">C10-C11</f>
+        <f t="shared" ref="C12:K12" si="83">C10-C11</f>
         <v>2278</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="83"/>
         <v>2750</v>
       </c>
       <c r="E12" s="2">
@@ -1499,15 +2338,15 @@
         <v>2945</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="83"/>
         <v>2512</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="83"/>
         <v>2336</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="83"/>
         <v>2796</v>
       </c>
       <c r="I12" s="2">
@@ -1518,7 +2357,7 @@
         <v>2581</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="83"/>
         <v>2690</v>
       </c>
       <c r="L12" s="2">
@@ -1526,19 +2365,19 @@
         <v>3186</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" ref="M12:P12" si="12">M10-M11</f>
+        <f t="shared" ref="M12:P12" si="84">M10-M11</f>
         <v>2951</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="84"/>
         <v>2733</v>
       </c>
       <c r="O12" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="84"/>
         <v>2884</v>
       </c>
       <c r="P12" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="84"/>
         <v>3105</v>
       </c>
       <c r="Q12" s="2">
@@ -1546,23 +2385,59 @@
         <v>3260.25</v>
       </c>
       <c r="R12" s="2">
-        <f t="shared" ref="R12:U12" si="13">Q12*1.05</f>
+        <f t="shared" ref="R12:U12" si="85">Q12*1.05</f>
         <v>3423.2625000000003</v>
       </c>
       <c r="S12" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="85"/>
         <v>3594.4256250000003</v>
       </c>
       <c r="T12" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="85"/>
         <v>3774.1469062500005</v>
       </c>
       <c r="U12" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="85"/>
         <v>3962.8542515625008</v>
       </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AC12" s="1">
+        <v>6228</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>6068</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>7253</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>8084</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>7620</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>8361</v>
+      </c>
+      <c r="AI12" s="1">
+        <v>8761</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>9593</v>
+      </c>
+      <c r="AK12" s="1">
+        <v>9115</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>10326</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>10873</v>
+      </c>
+      <c r="AN12" s="1">
+        <v>11560</v>
+      </c>
+    </row>
+    <row r="13" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1612,8 +2487,44 @@
       <c r="Q13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AC13" s="1">
+        <v>1133</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>1216</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>1126</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>1049</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>808</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>817</v>
+      </c>
+      <c r="AI13" s="1">
+        <v>747</v>
+      </c>
+      <c r="AJ13" s="1">
+        <v>705</v>
+      </c>
+      <c r="AK13" s="1">
+        <v>665</v>
+      </c>
+      <c r="AL13" s="1">
+        <v>1280</v>
+      </c>
+      <c r="AM13" s="1">
+        <v>1209</v>
+      </c>
+      <c r="AN13" s="1">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1662,17 +2573,53 @@
       <c r="Q14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AC14" s="1">
+        <v>5723</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>5582</v>
+      </c>
+      <c r="AE14" s="1">
+        <v>6477</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>6942</v>
+      </c>
+      <c r="AG14" s="1">
+        <v>7774</v>
+      </c>
+      <c r="AH14" s="1">
+        <v>8078</v>
+      </c>
+      <c r="AI14" s="1">
+        <v>21852</v>
+      </c>
+      <c r="AJ14" s="1">
+        <v>9828</v>
+      </c>
+      <c r="AK14" s="1">
+        <v>9341</v>
+      </c>
+      <c r="AL14" s="1">
+        <v>766</v>
+      </c>
+      <c r="AM14" s="1">
+        <v>6890</v>
+      </c>
+      <c r="AN14" s="1">
+        <v>3842</v>
+      </c>
+    </row>
+    <row r="15" spans="1:110" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" ref="C15:P15" si="14">C14-C16</f>
+        <f t="shared" ref="C15:P15" si="86">C14-C16</f>
         <v>395</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>604</v>
       </c>
       <c r="E15" s="2">
@@ -1684,43 +2631,43 @@
         <v>4711</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>468</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>627</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>-628</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>1969</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>516</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>759</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>-316</v>
       </c>
       <c r="N15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>949</v>
       </c>
       <c r="O15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>995</v>
       </c>
       <c r="P15" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="86"/>
         <v>994</v>
       </c>
       <c r="Q15" s="2">
@@ -1728,90 +2675,457 @@
         <v>1143.0999999999999</v>
       </c>
       <c r="R15" s="2">
-        <f t="shared" ref="R15:U15" si="15">Q15*1.15</f>
+        <f t="shared" ref="R15:U15" si="87">Q15*1.15</f>
         <v>1314.5649999999998</v>
       </c>
       <c r="S15" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="87"/>
         <v>1511.7497499999997</v>
       </c>
       <c r="T15" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="87"/>
         <v>1738.5122124999996</v>
       </c>
       <c r="U15" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="87"/>
         <v>1999.2890443749993</v>
       </c>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2">
+        <f t="shared" ref="Z15:AL15" si="88">AC14-AC16</f>
+        <v>1818</v>
+      </c>
+      <c r="AD15" s="2">
+        <f t="shared" si="88"/>
+        <v>2192</v>
+      </c>
+      <c r="AE15" s="2">
+        <f t="shared" si="88"/>
+        <v>2294</v>
+      </c>
+      <c r="AF15" s="2">
+        <f t="shared" si="88"/>
+        <v>2407</v>
+      </c>
+      <c r="AG15" s="2">
+        <f t="shared" si="88"/>
+        <v>2704</v>
+      </c>
+      <c r="AH15" s="2">
+        <f t="shared" si="88"/>
+        <v>2835</v>
+      </c>
+      <c r="AI15" s="2">
+        <f t="shared" si="88"/>
+        <v>7613</v>
+      </c>
+      <c r="AJ15" s="2">
+        <f t="shared" si="88"/>
+        <v>-394</v>
+      </c>
+      <c r="AK15" s="2">
+        <f t="shared" si="88"/>
+        <v>2378</v>
+      </c>
+      <c r="AL15" s="2">
+        <f t="shared" ref="AL15:AN15" si="89">AL14-AL16</f>
+        <v>2064</v>
+      </c>
+      <c r="AM15" s="2">
+        <f t="shared" si="89"/>
+        <v>2423</v>
+      </c>
+      <c r="AN15" s="2">
+        <f t="shared" si="89"/>
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="16" spans="1:110" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="5">
         <v>1121</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="5">
         <v>1997</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="5">
         <v>2600</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="5">
         <v>-4420</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="4">
         <v>1550</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="5">
         <v>1938</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="5">
         <v>952</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="5">
         <v>14</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="5">
         <v>1421</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="5">
         <v>2150</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="5">
         <v>-2720</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="5">
         <v>1624</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="5">
         <v>1959</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="5">
         <v>891</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q16" s="5">
         <f>Q7*0.26</f>
         <v>1749.9274000000003</v>
       </c>
-      <c r="R16" s="2">
-        <f t="shared" ref="R16:U16" si="16">R7*0.26</f>
+      <c r="R16" s="5">
+        <f t="shared" ref="R16:U16" si="90">R7*0.26</f>
         <v>1800.677242</v>
       </c>
-      <c r="S16" s="2">
-        <f t="shared" si="16"/>
+      <c r="S16" s="5">
+        <f t="shared" si="90"/>
         <v>1852.9150876600004</v>
       </c>
-      <c r="T16" s="2">
-        <f t="shared" si="16"/>
+      <c r="T16" s="5">
+        <f t="shared" si="90"/>
         <v>1906.6849106578006</v>
       </c>
-      <c r="U16" s="2">
-        <f t="shared" si="16"/>
+      <c r="U16" s="5">
+        <f t="shared" si="90"/>
         <v>1962.0319917228944</v>
       </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="AC16" s="4">
+        <v>3905</v>
+      </c>
+      <c r="AD16" s="4">
+        <v>3390</v>
+      </c>
+      <c r="AE16" s="4">
+        <v>4183</v>
+      </c>
+      <c r="AF16" s="4">
+        <v>4535</v>
+      </c>
+      <c r="AG16" s="4">
+        <v>5070</v>
+      </c>
+      <c r="AH16" s="4">
+        <v>5243</v>
+      </c>
+      <c r="AI16" s="4">
+        <v>14239</v>
+      </c>
+      <c r="AJ16" s="4">
+        <v>10222</v>
+      </c>
+      <c r="AK16" s="4">
+        <v>6963</v>
+      </c>
+      <c r="AL16" s="4">
+        <v>-1298</v>
+      </c>
+      <c r="AM16" s="4">
+        <v>4467</v>
+      </c>
+      <c r="AN16" s="4">
+        <v>2475</v>
+      </c>
+      <c r="AO16" s="5">
+        <f>AN16*(1+$AQ$26)</f>
+        <v>1361.25</v>
+      </c>
+      <c r="AP16" s="5">
+        <f t="shared" ref="AP16:DA16" si="91">AO16*(1+$AQ$26)</f>
+        <v>748.68750000000011</v>
+      </c>
+      <c r="AQ16" s="5">
+        <f t="shared" si="91"/>
+        <v>411.7781250000001</v>
+      </c>
+      <c r="AR16" s="5">
+        <f t="shared" si="91"/>
+        <v>226.47796875000009</v>
+      </c>
+      <c r="AS16" s="5">
+        <f t="shared" si="91"/>
+        <v>124.56288281250006</v>
+      </c>
+      <c r="AT16" s="5">
+        <f t="shared" si="91"/>
+        <v>68.509585546875044</v>
+      </c>
+      <c r="AU16" s="5">
+        <f t="shared" si="91"/>
+        <v>37.680272050781277</v>
+      </c>
+      <c r="AV16" s="5">
+        <f t="shared" si="91"/>
+        <v>20.724149627929705</v>
+      </c>
+      <c r="AW16" s="5">
+        <f t="shared" si="91"/>
+        <v>11.398282295361339</v>
+      </c>
+      <c r="AX16" s="5">
+        <f t="shared" si="91"/>
+        <v>6.2690552624487372</v>
+      </c>
+      <c r="AY16" s="5">
+        <f t="shared" si="91"/>
+        <v>3.4479803943468057</v>
+      </c>
+      <c r="AZ16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.8963892168907432</v>
+      </c>
+      <c r="BA16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.0430140692899088</v>
+      </c>
+      <c r="BB16" s="5">
+        <f t="shared" si="91"/>
+        <v>0.57365773810944987</v>
+      </c>
+      <c r="BC16" s="5">
+        <f t="shared" si="91"/>
+        <v>0.31551175596019743</v>
+      </c>
+      <c r="BD16" s="5">
+        <f t="shared" si="91"/>
+        <v>0.1735314657781086</v>
+      </c>
+      <c r="BE16" s="5">
+        <f t="shared" si="91"/>
+        <v>9.5442306177959735E-2</v>
+      </c>
+      <c r="BF16" s="5">
+        <f t="shared" si="91"/>
+        <v>5.2493268397877858E-2</v>
+      </c>
+      <c r="BG16" s="5">
+        <f t="shared" si="91"/>
+        <v>2.8871297618832826E-2</v>
+      </c>
+      <c r="BH16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.5879213690358055E-2</v>
+      </c>
+      <c r="BI16" s="5">
+        <f t="shared" si="91"/>
+        <v>8.7335675296969315E-3</v>
+      </c>
+      <c r="BJ16" s="5">
+        <f t="shared" si="91"/>
+        <v>4.8034621413333128E-3</v>
+      </c>
+      <c r="BK16" s="5">
+        <f t="shared" si="91"/>
+        <v>2.641904177733322E-3</v>
+      </c>
+      <c r="BL16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.4530472977533273E-3</v>
+      </c>
+      <c r="BM16" s="5">
+        <f t="shared" si="91"/>
+        <v>7.9917601376433003E-4</v>
+      </c>
+      <c r="BN16" s="5">
+        <f t="shared" si="91"/>
+        <v>4.3954680757038158E-4</v>
+      </c>
+      <c r="BO16" s="5">
+        <f t="shared" si="91"/>
+        <v>2.417507441637099E-4</v>
+      </c>
+      <c r="BP16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.3296290929004046E-4</v>
+      </c>
+      <c r="BQ16" s="5">
+        <f t="shared" si="91"/>
+        <v>7.3129600109522253E-5</v>
+      </c>
+      <c r="BR16" s="5">
+        <f t="shared" si="91"/>
+        <v>4.0221280060237242E-5</v>
+      </c>
+      <c r="BS16" s="5">
+        <f t="shared" si="91"/>
+        <v>2.2121704033130484E-5</v>
+      </c>
+      <c r="BT16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.2166937218221767E-5</v>
+      </c>
+      <c r="BU16" s="5">
+        <f t="shared" si="91"/>
+        <v>6.6918154700219725E-6</v>
+      </c>
+      <c r="BV16" s="5">
+        <f t="shared" si="91"/>
+        <v>3.680498508512085E-6</v>
+      </c>
+      <c r="BW16" s="5">
+        <f t="shared" si="91"/>
+        <v>2.0242741796816471E-6</v>
+      </c>
+      <c r="BX16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.1133507988249059E-6</v>
+      </c>
+      <c r="BY16" s="5">
+        <f t="shared" si="91"/>
+        <v>6.1234293935369836E-7</v>
+      </c>
+      <c r="BZ16" s="5">
+        <f t="shared" si="91"/>
+        <v>3.3678861664453415E-7</v>
+      </c>
+      <c r="CA16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.8523373915449379E-7</v>
+      </c>
+      <c r="CB16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.018785565349716E-7</v>
+      </c>
+      <c r="CC16" s="5">
+        <f t="shared" si="91"/>
+        <v>5.6033206094234383E-8</v>
+      </c>
+      <c r="CD16" s="5">
+        <f t="shared" si="91"/>
+        <v>3.0818263351828912E-8</v>
+      </c>
+      <c r="CE16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.6950044843505902E-8</v>
+      </c>
+      <c r="CF16" s="5">
+        <f t="shared" si="91"/>
+        <v>9.3225246639282475E-9</v>
+      </c>
+      <c r="CG16" s="5">
+        <f t="shared" si="91"/>
+        <v>5.1273885651605365E-9</v>
+      </c>
+      <c r="CH16" s="5">
+        <f t="shared" si="91"/>
+        <v>2.8200637108382951E-9</v>
+      </c>
+      <c r="CI16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.5510350409610624E-9</v>
+      </c>
+      <c r="CJ16" s="5">
+        <f t="shared" si="91"/>
+        <v>8.5306927252858441E-10</v>
+      </c>
+      <c r="CK16" s="5">
+        <f t="shared" si="91"/>
+        <v>4.691880998907215E-10</v>
+      </c>
+      <c r="CL16" s="5">
+        <f t="shared" si="91"/>
+        <v>2.5805345493989684E-10</v>
+      </c>
+      <c r="CM16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.4192940021694327E-10</v>
+      </c>
+      <c r="CN16" s="5">
+        <f t="shared" si="91"/>
+        <v>7.8061170119318803E-11</v>
+      </c>
+      <c r="CO16" s="5">
+        <f t="shared" si="91"/>
+        <v>4.2933643565625344E-11</v>
+      </c>
+      <c r="CP16" s="5">
+        <f t="shared" si="91"/>
+        <v>2.3613503961093941E-11</v>
+      </c>
+      <c r="CQ16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.2987427178601669E-11</v>
+      </c>
+      <c r="CR16" s="5">
+        <f t="shared" si="91"/>
+        <v>7.1430849482309187E-12</v>
+      </c>
+      <c r="CS16" s="5">
+        <f t="shared" si="91"/>
+        <v>3.9286967215270056E-12</v>
+      </c>
+      <c r="CT16" s="5">
+        <f t="shared" si="91"/>
+        <v>2.1607831968398532E-12</v>
+      </c>
+      <c r="CU16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.1884307582619194E-12</v>
+      </c>
+      <c r="CV16" s="5">
+        <f t="shared" si="91"/>
+        <v>6.5363691704405567E-13</v>
+      </c>
+      <c r="CW16" s="5">
+        <f t="shared" si="91"/>
+        <v>3.5950030437423064E-13</v>
+      </c>
+      <c r="CX16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.9772516740582688E-13</v>
+      </c>
+      <c r="CY16" s="5">
+        <f t="shared" si="91"/>
+        <v>1.0874884207320479E-13</v>
+      </c>
+      <c r="CZ16" s="5">
+        <f t="shared" si="91"/>
+        <v>5.9811863140262636E-14</v>
+      </c>
+      <c r="DA16" s="5">
+        <f t="shared" si="91"/>
+        <v>3.2896524727144453E-14</v>
+      </c>
+      <c r="DB16" s="5">
+        <f t="shared" ref="DB16:DF16" si="92">DA16*(1+$AQ$26)</f>
+        <v>1.8093088599929452E-14</v>
+      </c>
+      <c r="DC16" s="5">
+        <f t="shared" si="92"/>
+        <v>9.951198729961199E-15</v>
+      </c>
+      <c r="DD16" s="5">
+        <f t="shared" si="92"/>
+        <v>5.4731593014786599E-15</v>
+      </c>
+      <c r="DE16" s="5">
+        <f t="shared" si="92"/>
+        <v>3.0102376158132633E-15</v>
+      </c>
+      <c r="DF16" s="5">
+        <f t="shared" si="92"/>
+        <v>1.6556306886972949E-15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:43" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1862,80 +3176,116 @@
         <v>1.0024602810512533</v>
       </c>
       <c r="R17" s="6">
-        <f t="shared" ref="R17:U17" si="17">R16/R18</f>
+        <f t="shared" ref="R17:U17" si="93">R16/R18</f>
         <v>1.0745132758185638</v>
       </c>
       <c r="S17" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="93"/>
         <v>1.151755233980176</v>
       </c>
       <c r="T17" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="93"/>
         <v>1.2345604884220922</v>
       </c>
       <c r="U17" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="93"/>
         <v>1.3233304178791043</v>
       </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="AC17" s="1">
+        <v>1.87</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>1.64</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AG17" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="AH17" s="1">
+        <v>2.67</v>
+      </c>
+      <c r="AI17" s="1">
+        <v>7.28</v>
+      </c>
+      <c r="AJ17" s="1">
+        <v>5.31</v>
+      </c>
+      <c r="AK17" s="1">
+        <v>3.69</v>
+      </c>
+      <c r="AL17" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="AM17" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="AN17" s="1">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:43" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="2">
-        <f>C16/C17</f>
+        <f t="shared" ref="C18:P18" si="94">C16/C17</f>
         <v>1868.3333333333335</v>
       </c>
       <c r="D18" s="2">
-        <f>D16/D17</f>
+        <f t="shared" si="94"/>
         <v>1866.3551401869158</v>
       </c>
       <c r="E18" s="2">
-        <f>E16/E17</f>
+        <f t="shared" si="94"/>
         <v>1870.5035971223024</v>
       </c>
       <c r="F18" s="2">
-        <f>F16/F17</f>
+        <f t="shared" si="94"/>
         <v>1872.8813559322034</v>
       </c>
       <c r="G18" s="2">
-        <f>G16/G17</f>
+        <f t="shared" si="94"/>
         <v>1867.4698795180723</v>
       </c>
       <c r="H18" s="2">
-        <f>H16/H17</f>
+        <f t="shared" si="94"/>
         <v>1863.4615384615383</v>
       </c>
       <c r="I18" s="2">
-        <f>I16/I17</f>
+        <f t="shared" si="94"/>
         <v>1866.6666666666667</v>
       </c>
       <c r="J18" s="2">
-        <f>J16/J17</f>
+        <f t="shared" si="94"/>
         <v>700</v>
       </c>
       <c r="K18" s="2">
-        <f>K16/K17</f>
+        <f t="shared" si="94"/>
         <v>1845.4545454545455</v>
       </c>
       <c r="L18" s="2">
-        <f>L16/L17</f>
+        <f t="shared" si="94"/>
         <v>1853.4482758620691</v>
       </c>
       <c r="M18" s="2">
-        <f>M16/M17</f>
+        <f t="shared" si="94"/>
         <v>1837.8378378378379</v>
       </c>
       <c r="N18" s="2">
-        <f>N16/N17</f>
+        <f t="shared" si="94"/>
         <v>1489.9082568807339</v>
       </c>
       <c r="O18" s="2">
-        <f>O16/O17</f>
+        <f t="shared" si="94"/>
         <v>1813.8888888888887</v>
       </c>
       <c r="P18" s="2">
-        <f>P16/P17</f>
+        <f t="shared" si="94"/>
         <v>1818.3673469387757</v>
       </c>
       <c r="Q18" s="2">
@@ -1943,23 +3293,30 @@
         <v>1745.6326530612246</v>
       </c>
       <c r="R18" s="2">
-        <f t="shared" ref="R18:U18" si="18">Q18*0.96</f>
+        <f t="shared" ref="R18:U18" si="95">Q18*0.96</f>
         <v>1675.8073469387755</v>
       </c>
       <c r="S18" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="95"/>
         <v>1608.7750530612243</v>
       </c>
       <c r="T18" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="95"/>
         <v>1544.4240509387753</v>
       </c>
       <c r="U18" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="95"/>
         <v>1482.6470889012242</v>
       </c>
-    </row>
-    <row r="20" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="2"/>
+      <c r="AL18" s="2"/>
+      <c r="AM18" s="2"/>
+      <c r="AN18" s="2"/>
+    </row>
+    <row r="20" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>50</v>
       </c>
@@ -1969,43 +3326,87 @@
         <v>0.12988628287135739</v>
       </c>
       <c r="H20" s="9">
-        <f t="shared" ref="H20:P20" si="19">H7/D7-1</f>
+        <f t="shared" ref="H20:P20" si="96">H7/D7-1</f>
         <v>-3.8072216346880183E-2</v>
       </c>
       <c r="I20" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="96"/>
         <v>3.8943990665110784E-2</v>
       </c>
       <c r="J20" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="96"/>
         <v>4.9442317296487515E-2</v>
       </c>
       <c r="K20" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="96"/>
         <v>-5.0794150023588669E-2</v>
       </c>
       <c r="L20" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="96"/>
         <v>8.9367048845610197E-2</v>
       </c>
       <c r="M20" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="96"/>
         <v>-4.7311526042397856E-2</v>
       </c>
       <c r="N20" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="96"/>
         <v>-7.7728426395938799E-3</v>
       </c>
       <c r="O20" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="96"/>
         <v>-2.3856858846918461E-2</v>
       </c>
       <c r="P20" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="96"/>
         <v>-5.6660899653979246E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD20" s="9">
+        <f t="shared" ref="AD20:AJ20" si="97">AD7/AC7-1</f>
+        <v>-2.310881254361119E-2</v>
+      </c>
+      <c r="AE20" s="9">
+        <f t="shared" si="97"/>
+        <v>3.4369747899159586E-2</v>
+      </c>
+      <c r="AF20" s="9">
+        <f t="shared" si="97"/>
+        <v>-6.1743439759525121E-3</v>
+      </c>
+      <c r="AG20" s="9">
+        <f t="shared" si="97"/>
+        <v>2.2888907054687824E-3</v>
+      </c>
+      <c r="AH20" s="9">
+        <f t="shared" si="97"/>
+        <v>3.7191093711768985E-2</v>
+      </c>
+      <c r="AI20" s="9">
+        <f t="shared" si="97"/>
+        <v>1.2188409216010054E-2</v>
+      </c>
+      <c r="AJ20" s="9">
+        <f t="shared" ref="AJ20:AM20" si="98">AJ7/AI7-1</f>
+        <v>-6.525792417650722E-3</v>
+      </c>
+      <c r="AK20" s="9">
+        <f t="shared" si="98"/>
+        <v>-8.2890209571473417E-3</v>
+      </c>
+      <c r="AL20" s="9">
+        <f t="shared" si="98"/>
+        <v>-1.0014193344898281E-2</v>
+      </c>
+      <c r="AM20" s="9">
+        <f t="shared" si="98"/>
+        <v>4.153723616089211E-2</v>
+      </c>
+      <c r="AN20" s="9">
+        <f>AN7/AM7-1</f>
+        <v>-5.3531143654648172E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>51</v>
       </c>
@@ -2014,7 +3415,7 @@
         <v>7.0184790334044067E-2</v>
       </c>
       <c r="D21" s="9">
-        <f t="shared" ref="D21:P21" si="20">D15/D7</f>
+        <f t="shared" ref="D21:P21" si="99">D15/D7</f>
         <v>9.1252455053633483E-2</v>
       </c>
       <c r="E21" s="9">
@@ -2026,11 +3427,11 @@
         <v>0.78425170634260033</v>
       </c>
       <c r="G21" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="99"/>
         <v>7.3596477433558738E-2</v>
       </c>
       <c r="H21" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="99"/>
         <v>9.8476519553950051E-2</v>
       </c>
       <c r="I21" s="9">
@@ -2038,15 +3439,15 @@
         <v>8.8165098975150916E-2</v>
       </c>
       <c r="J21" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="99"/>
         <v>0.31234137055837563</v>
       </c>
       <c r="K21" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="99"/>
         <v>8.5487077534791248E-2</v>
       </c>
       <c r="L21" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="99"/>
         <v>0.10942906574394463</v>
       </c>
       <c r="M21" s="9">
@@ -2054,133 +3455,229 @@
         <v>4.6566460359563806E-2</v>
       </c>
       <c r="N21" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="99"/>
         <v>0.15171862509992007</v>
       </c>
       <c r="O21" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="99"/>
         <v>0.16887304820095045</v>
       </c>
       <c r="P21" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="99"/>
         <v>0.15191808039125784</v>
       </c>
-    </row>
-    <row r="22" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC21" s="9">
+        <f t="shared" ref="AC21:AJ21" si="100">AC15/AC14</f>
+        <v>0.31766556002096802</v>
+      </c>
+      <c r="AD21" s="9">
+        <f t="shared" si="100"/>
+        <v>0.39269079183088501</v>
+      </c>
+      <c r="AE21" s="9">
+        <f t="shared" si="100"/>
+        <v>0.35417631619576967</v>
+      </c>
+      <c r="AF21" s="9">
+        <f t="shared" si="100"/>
+        <v>0.34673004897723997</v>
+      </c>
+      <c r="AG21" s="9">
+        <f t="shared" si="100"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="AH21" s="9">
+        <f t="shared" si="100"/>
+        <v>0.35095320623916809</v>
+      </c>
+      <c r="AI21" s="9">
+        <f t="shared" si="100"/>
+        <v>0.34838916346329857</v>
+      </c>
+      <c r="AJ21" s="9">
+        <f t="shared" ref="AI21:AN21" si="101">AJ15/AJ14</f>
+        <v>-4.0089540089540091E-2</v>
+      </c>
+      <c r="AK21" s="9">
+        <f t="shared" si="101"/>
+        <v>0.25457659779466868</v>
+      </c>
+      <c r="AL21" s="9">
+        <f t="shared" si="101"/>
+        <v>2.6945169712793735</v>
+      </c>
+      <c r="AM21" s="9">
+        <f t="shared" si="101"/>
+        <v>0.3516690856313498</v>
+      </c>
+      <c r="AN21" s="9">
+        <f>AN15/AN14</f>
+        <v>0.35580426861009889</v>
+      </c>
+    </row>
+    <row r="22" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C22" s="9">
-        <f t="shared" ref="C22:P22" si="21">C9/C7</f>
+        <f t="shared" ref="C22:O22" si="102">C9/C7</f>
         <v>0.22014925373134328</v>
       </c>
       <c r="D22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.21544039885179031</v>
       </c>
       <c r="E22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.21061843640606767</v>
       </c>
       <c r="F22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.200599300815715</v>
       </c>
       <c r="G22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.20647900613303979</v>
       </c>
       <c r="H22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.20496309093764725</v>
       </c>
       <c r="I22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.20286396181384247</v>
       </c>
       <c r="J22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.19812817258883247</v>
       </c>
       <c r="K22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.19151756129887343</v>
       </c>
       <c r="L22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.19059976931949249</v>
       </c>
       <c r="M22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.18493958149130563</v>
       </c>
       <c r="N22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.18689048760991206</v>
       </c>
       <c r="O22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="102"/>
         <v>0.18211133740665308</v>
       </c>
       <c r="P22" s="9">
         <f>P9/P7</f>
         <v>0.17866422130521167</v>
       </c>
-    </row>
-    <row r="23" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC22" s="9">
+        <f>AC10/AC7</f>
+        <v>0.37712925337602099</v>
+      </c>
+      <c r="AD22" s="9">
+        <f t="shared" ref="AD22:AN22" si="103">AD10/AD7</f>
+        <v>0.37558823529411767</v>
+      </c>
+      <c r="AE22" s="9">
+        <f t="shared" si="103"/>
+        <v>0.38845560159233083</v>
+      </c>
+      <c r="AF22" s="9">
+        <f t="shared" si="103"/>
+        <v>0.42740946619798903</v>
+      </c>
+      <c r="AG22" s="9">
+        <f t="shared" si="103"/>
+        <v>0.41432183345567247</v>
+      </c>
+      <c r="AH22" s="9">
+        <f t="shared" si="103"/>
+        <v>0.43697412911850281</v>
+      </c>
+      <c r="AI22" s="9">
+        <f t="shared" si="103"/>
+        <v>0.449502796768179</v>
+      </c>
+      <c r="AJ22" s="9">
+        <f t="shared" si="103"/>
+        <v>0.46774319674695025</v>
+      </c>
+      <c r="AK22" s="9">
+        <f t="shared" si="103"/>
+        <v>0.48312568995426591</v>
+      </c>
+      <c r="AL22" s="9">
+        <f t="shared" si="103"/>
+        <v>0.50621266427718037</v>
+      </c>
+      <c r="AM22" s="9">
+        <f t="shared" si="103"/>
+        <v>0.49795434558176882</v>
+      </c>
+      <c r="AN22" s="9">
+        <f t="shared" si="103"/>
+        <v>0.53788490370199515</v>
+      </c>
+    </row>
+    <row r="23" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="9">
-        <f t="shared" ref="C23:P23" si="22">C8/C7</f>
+        <f t="shared" ref="C23:O23" si="104">C8/C7</f>
         <v>0.31236673773987206</v>
       </c>
       <c r="D23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.28312433902402173</v>
       </c>
       <c r="E23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.27931738623103852</v>
       </c>
       <c r="F23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.25603462626935242</v>
       </c>
       <c r="G23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.34172039628872464</v>
       </c>
       <c r="H23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.27878121564316005</v>
       </c>
       <c r="I23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.27530534886985819</v>
       </c>
       <c r="J23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.30282360406091369</v>
       </c>
       <c r="K23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.26640159045725648</v>
       </c>
       <c r="L23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.27133794694348329</v>
       </c>
       <c r="M23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.27379899793692897</v>
       </c>
       <c r="N23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.28313349320543563</v>
       </c>
       <c r="O23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="104"/>
         <v>0.24541751527494909</v>
       </c>
       <c r="P23" s="9">
@@ -2188,60 +3685,60 @@
         <v>0.2610423353201895</v>
       </c>
     </row>
-    <row r="24" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="9">
-        <f t="shared" ref="C24:P24" si="23">C11/C7</f>
+        <f t="shared" ref="C24:O24" si="105">C11/C7</f>
         <v>9.4705046197583506E-2</v>
       </c>
       <c r="D24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>8.5964647227677896E-2</v>
       </c>
       <c r="E24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>8.051341890315053E-2</v>
       </c>
       <c r="F24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>9.522224071916098E-2</v>
       </c>
       <c r="G24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>8.4447240132096243E-2</v>
       </c>
       <c r="H24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>7.7116381341291035E-2</v>
       </c>
       <c r="I24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>7.8197388740699147E-2</v>
       </c>
       <c r="J24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>9.0260152284263956E-2</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>9.6421471172962223E-2</v>
       </c>
       <c r="L24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>7.8719723183391002E-2</v>
       </c>
       <c r="M24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>0.10639552018862364</v>
       </c>
       <c r="N24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>9.3045563549160673E-2</v>
       </c>
       <c r="O24" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="105"/>
         <v>8.2993890020366598E-2</v>
       </c>
       <c r="P24" s="9">
@@ -2249,7 +3746,7 @@
         <v>8.5740486015589173E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="s">
         <v>32</v>
       </c>
@@ -2258,59 +3755,65 @@
         <v>0.26936744847192606</v>
       </c>
       <c r="D25" s="9">
-        <f t="shared" ref="D25:P25" si="24">D14/D7</f>
+        <f t="shared" ref="D25:P25" si="106">D14/D7</f>
         <v>0.39295966158029916</v>
       </c>
       <c r="E25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>0.31038506417736289</v>
       </c>
       <c r="F25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>4.8443482603629101E-2</v>
       </c>
       <c r="G25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>0.31734549457461864</v>
       </c>
       <c r="H25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>0.40285848908434113</v>
       </c>
       <c r="I25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>4.5486452337498248E-2</v>
       </c>
       <c r="J25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>0.31456218274111675</v>
       </c>
       <c r="K25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>0.32090788601722997</v>
       </c>
       <c r="L25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>0.41940599769319492</v>
       </c>
       <c r="M25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>-0.44739168877099911</v>
       </c>
       <c r="N25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>0.41135091926458833</v>
       </c>
       <c r="O25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>0.50135777325186692</v>
       </c>
       <c r="P25" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="106"/>
         <v>0.28809414641601711</v>
       </c>
-    </row>
-    <row r="26" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AP25" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ25" s="19">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="s">
         <v>55</v>
       </c>
@@ -2319,43 +3822,49 @@
         <v>-4.62151908257602E-4</v>
       </c>
       <c r="H26" s="9">
-        <f t="shared" ref="H26:P26" si="25">H18/D18-1</f>
+        <f t="shared" ref="H26:P26" si="107">H18/D18-1</f>
         <v>-1.5504025268672228E-3</v>
       </c>
       <c r="I26" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="107"/>
         <v>-2.0512820512821328E-3</v>
       </c>
       <c r="J26" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="107"/>
         <v>-0.62624434389140271</v>
       </c>
       <c r="K26" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="107"/>
         <v>-1.1788856304985273E-2</v>
       </c>
       <c r="L26" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="107"/>
         <v>-5.3734742535851421E-3</v>
       </c>
       <c r="M26" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="107"/>
         <v>-1.5444015444015413E-2</v>
       </c>
       <c r="N26" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="107"/>
         <v>1.1284403669724772</v>
       </c>
       <c r="O26" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="107"/>
         <v>-1.7104542966612013E-2</v>
       </c>
       <c r="P26" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="107"/>
         <v>-1.8927384907451383E-2</v>
       </c>
-    </row>
-    <row r="27" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AP26" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ26" s="21">
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="10" t="s">
         <v>56</v>
       </c>
@@ -2364,43 +3873,50 @@
         <v>0.18481012658227858</v>
       </c>
       <c r="H27" s="9">
-        <f t="shared" ref="H27:P27" si="26">H15/D15-1</f>
+        <f t="shared" ref="H27:P27" si="108">H15/D15-1</f>
         <v>3.8079470198675525E-2</v>
       </c>
       <c r="I27" s="9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="108"/>
         <v>0.33050847457627119</v>
       </c>
       <c r="J27" s="9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="108"/>
         <v>-0.58204202929314364</v>
       </c>
       <c r="K27" s="9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="108"/>
         <v>0.10256410256410264</v>
       </c>
       <c r="L27" s="9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="108"/>
         <v>0.21052631578947367</v>
       </c>
       <c r="M27" s="9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="108"/>
         <v>-0.49681528662420382</v>
       </c>
       <c r="N27" s="9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="108"/>
         <v>-0.51802945657694255</v>
       </c>
       <c r="O27" s="9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="108"/>
         <v>0.92829457364341095</v>
       </c>
       <c r="P27" s="9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="108"/>
         <v>0.30961791831357055</v>
       </c>
-    </row>
-    <row r="28" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AP27" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ27" s="23">
+        <f>NPV(AQ25,AO16:DF16)</f>
+        <v>2592.8571428571422</v>
+      </c>
+    </row>
+    <row r="28" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="10" t="s">
         <v>57</v>
       </c>
@@ -2409,160 +3925,311 @@
         <v>0.13596757852076991</v>
       </c>
       <c r="H28" s="9">
-        <f t="shared" ref="H28:P28" si="27">H3/D3-1</f>
+        <f t="shared" ref="H28:P28" si="109">H3/D3-1</f>
         <v>-4.2713138561421449E-2</v>
       </c>
       <c r="I28" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="109"/>
         <v>4.3643577450818372E-2</v>
       </c>
       <c r="J28" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="109"/>
         <v>7.9085094010467039E-2</v>
       </c>
       <c r="K28" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="109"/>
         <v>-6.3503389225829432E-2</v>
       </c>
       <c r="L28" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="109"/>
         <v>7.977868998750659E-2</v>
       </c>
       <c r="M28" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="109"/>
         <v>-5.3540313638523629E-2</v>
       </c>
       <c r="N28" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="109"/>
         <v>4.3111190946649725E-3</v>
       </c>
       <c r="O28" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="109"/>
         <v>2.8571428571428914E-3</v>
       </c>
       <c r="P28" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="109"/>
         <v>-2.9256198347107465E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD28" s="9">
+        <f>AD3/AC3-1</f>
+        <v>-9.9589923842999806E-3</v>
+      </c>
+      <c r="AE28" s="9">
+        <f>AE3/AD3-1</f>
+        <v>1.1197086936731937E-2</v>
+      </c>
+      <c r="AF28" s="9">
+        <f t="shared" ref="AF28:AN28" si="110">AF3/AE3-1</f>
+        <v>-1.566438602808784E-2</v>
+      </c>
+      <c r="AG28" s="9">
+        <f t="shared" si="110"/>
+        <v>3.2467532467532756E-3</v>
+      </c>
+      <c r="AH28" s="9">
+        <f t="shared" si="110"/>
+        <v>3.8880532385249911E-2</v>
+      </c>
+      <c r="AI28" s="9">
+        <f t="shared" si="110"/>
+        <v>2.5886275886275456E-3</v>
+      </c>
+      <c r="AJ28" s="9">
+        <f t="shared" si="110"/>
+        <v>-9.4087786092512671E-3</v>
+      </c>
+      <c r="AK28" s="9">
+        <f t="shared" si="110"/>
+        <v>-1.4976144195087526E-2</v>
+      </c>
+      <c r="AL28" s="9">
+        <f t="shared" si="110"/>
+        <v>-1.3499573933713038E-2</v>
+      </c>
+      <c r="AM28" s="9">
+        <f t="shared" si="110"/>
+        <v>4.9690852882342318E-2</v>
+      </c>
+      <c r="AN28" s="9">
+        <f t="shared" si="110"/>
+        <v>-9.6582788340768833E-3</v>
+      </c>
+      <c r="AP28" s="22"/>
+      <c r="AQ28" s="24">
+        <f>AQ27/Main!M2</f>
+        <v>58.635394456289966</v>
+      </c>
+    </row>
+    <row r="29" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G29" s="9">
-        <f t="shared" ref="G29:P29" si="28">G4/C4-1</f>
+        <f t="shared" ref="G29:P29" si="111">G4/C4-1</f>
         <v>0.11296296296296293</v>
       </c>
       <c r="H29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="111"/>
         <v>9.6345514950166189E-2</v>
       </c>
       <c r="I29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="111"/>
         <v>3.2258064516129004E-2</v>
       </c>
       <c r="J29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="111"/>
         <v>4.4628099173553704E-2</v>
       </c>
       <c r="K29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="111"/>
         <v>4.1597337770382659E-2</v>
       </c>
       <c r="L29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="111"/>
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="M29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="111"/>
         <v>-2.1874999999999978E-2</v>
       </c>
       <c r="N29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="111"/>
         <v>4.9050632911392444E-2</v>
       </c>
       <c r="O29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="111"/>
         <v>-2.0766773162939289E-2</v>
       </c>
       <c r="P29" s="9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="111"/>
         <v>-4.0404040404040442E-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD29" s="9">
+        <f>AD4/AC4-1</f>
+        <v>4.8324742268041287E-2</v>
+      </c>
+      <c r="AE29" s="9">
+        <f t="shared" ref="AE29:AN29" si="112">AE4/AD4-1</f>
+        <v>3.9336201598033194E-2</v>
+      </c>
+      <c r="AF29" s="9">
+        <f t="shared" si="112"/>
+        <v>5.1448846836191553E-2</v>
+      </c>
+      <c r="AG29" s="9">
+        <f t="shared" si="112"/>
+        <v>1.7435320584926917E-2</v>
+      </c>
+      <c r="AH29" s="9">
+        <f t="shared" si="112"/>
+        <v>3.8695411829740234E-2</v>
+      </c>
+      <c r="AI29" s="9">
+        <f t="shared" si="112"/>
+        <v>9.1538052155401894E-2</v>
+      </c>
+      <c r="AJ29" s="9">
+        <f t="shared" si="112"/>
+        <v>5.0706972208678591E-2</v>
+      </c>
+      <c r="AK29" s="9">
+        <f t="shared" si="112"/>
+        <v>4.9651972157772617E-2</v>
+      </c>
+      <c r="AL29" s="9">
+        <f t="shared" si="112"/>
+        <v>4.6419098143235971E-2</v>
+      </c>
+      <c r="AM29" s="9">
+        <f t="shared" si="112"/>
+        <v>7.013096746937042E-2</v>
+      </c>
+      <c r="AN29" s="9">
+        <f t="shared" si="112"/>
+        <v>2.9609159099881488E-2</v>
+      </c>
+      <c r="AP29" s="22"/>
+      <c r="AQ29" s="25"/>
+    </row>
+    <row r="30" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="10"/>
       <c r="Q30" s="11"/>
       <c r="R30" s="12"/>
       <c r="S30" s="12"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="AA30" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD30" s="9">
+        <f t="shared" ref="AD30:AN30" si="113">AD16/AC16-1</f>
+        <v>-0.13188220230473746</v>
+      </c>
+      <c r="AE30" s="9">
+        <f t="shared" si="113"/>
+        <v>0.2339233038348083</v>
+      </c>
+      <c r="AF30" s="9">
+        <f t="shared" si="113"/>
+        <v>8.4150131484580504E-2</v>
+      </c>
+      <c r="AG30" s="9">
+        <f t="shared" si="113"/>
+        <v>0.11797133406835725</v>
+      </c>
+      <c r="AH30" s="9">
+        <f t="shared" si="113"/>
+        <v>3.4122287968441745E-2</v>
+      </c>
+      <c r="AI30" s="9">
+        <f t="shared" si="113"/>
+        <v>1.7158115582681672</v>
+      </c>
+      <c r="AJ30" s="9">
+        <f t="shared" si="113"/>
+        <v>-0.28211250790083575</v>
+      </c>
+      <c r="AK30" s="9">
+        <f t="shared" si="113"/>
+        <v>-0.31882214830757194</v>
+      </c>
+      <c r="AL30" s="9">
+        <f t="shared" si="113"/>
+        <v>-1.1864139020537126</v>
+      </c>
+      <c r="AM30" s="9">
+        <f t="shared" si="113"/>
+        <v>-4.4414483821263477</v>
+      </c>
+      <c r="AN30" s="9">
+        <f>AN16/AM16-1</f>
+        <v>-0.44593687038280727</v>
+      </c>
+      <c r="AP30" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ30" s="33">
+        <f>AQ28/Main!M2-1</f>
+        <v>0.32599263808887313</v>
+      </c>
+    </row>
+    <row r="31" spans="2:43" x14ac:dyDescent="0.2">
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
       <c r="S31" s="13"/>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:43" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" ref="C32:P32" si="29">C33-C48</f>
+        <f t="shared" ref="C32:P32" si="114">C33-C48</f>
         <v>3352</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>1796</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>1604</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>2117</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>5616</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>4826</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>2957</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>4945</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>5792</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>1877</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>2957</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>4544</v>
       </c>
       <c r="O32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>5353</v>
       </c>
       <c r="P32" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="114"/>
         <v>2567</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="AP32" s="27"/>
+      <c r="AQ32" s="27"/>
+    </row>
+    <row r="33" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
@@ -2608,8 +4275,14 @@
       <c r="P33" s="2">
         <v>2567</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="AQ33" s="27">
+        <v>2.0400000000000001E-2</v>
+      </c>
+      <c r="AR33" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>41</v>
       </c>
@@ -2656,7 +4329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>42</v>
       </c>
@@ -2703,7 +4376,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -2750,7 +4423,7 @@
         <v>4345</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
@@ -2797,7 +4470,7 @@
         <v>376746</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
@@ -2844,7 +4517,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
@@ -2891,7 +4564,7 @@
         <v>25046</v>
       </c>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>43</v>
       </c>
@@ -2938,7 +4611,7 @@
         <v>39149</v>
       </c>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>39</v>
       </c>
@@ -2985,7 +4658,7 @@
         <v>2403</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>44</v>
       </c>
@@ -3038,6 +4711,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="AC7" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MO & MU update
</commit_message>
<xml_diff>
--- a/MO.xlsx
+++ b/MO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738113E5-F816-4A1A-B483-24811E92445A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136EA075-45FA-4076-865C-5FC9BE4C00C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -815,14 +815,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="9.140625" style="1"/>
+    <col min="1" max="11" width="9.109375" style="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L2" s="1" t="s">
         <v>0</v>
       </c>
@@ -830,7 +830,7 @@
         <v>44.22</v>
       </c>
     </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C3" s="16" t="s">
         <v>64</v>
       </c>
@@ -841,7 +841,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>67</v>
       </c>
@@ -853,7 +853,7 @@
         <v>79596</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
         <v>68</v>
       </c>
@@ -864,7 +864,7 @@
         <v>2567</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
@@ -872,7 +872,7 @@
         <v>2634</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L7" s="1" t="s">
         <v>5</v>
       </c>
@@ -881,29 +881,29 @@
         <v>79663</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C13" s="18" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="28"/>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C14" s="20" t="s">
         <v>65</v>
       </c>
       <c r="D14" s="29"/>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C15" s="20" t="s">
         <v>66</v>
       </c>
       <c r="D15" s="29"/>
     </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C16" s="30"/>
       <c r="D16" s="29"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="31"/>
       <c r="D17" s="32"/>
     </row>
@@ -921,23 +921,23 @@
       <pane xSplit="2" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AR30" sqref="AR30"/>
+      <selection pane="bottomRight" activeCell="AK17" sqref="AK17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.109375" style="1"/>
+    <col min="10" max="10" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.109375" style="1"/>
+    <col min="14" max="14" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -984,7 +984,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="2" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:110" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>2091</v>
       </c>
     </row>
-    <row r="3" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1437,44 +1437,44 @@
         <f t="shared" si="71"/>
         <v>6808.4166383639013</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AC3" s="2">
         <v>22191</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="AD3" s="2">
         <v>21970</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AE3" s="2">
         <v>22216</v>
       </c>
-      <c r="AF3" s="1">
+      <c r="AF3" s="2">
         <v>21868</v>
       </c>
-      <c r="AG3" s="1">
+      <c r="AG3" s="2">
         <v>21939</v>
       </c>
-      <c r="AH3" s="1">
+      <c r="AH3" s="2">
         <v>22792</v>
       </c>
-      <c r="AI3" s="1">
+      <c r="AI3" s="2">
         <v>22851</v>
       </c>
-      <c r="AJ3" s="1">
+      <c r="AJ3" s="2">
         <v>22636</v>
       </c>
-      <c r="AK3" s="1">
+      <c r="AK3" s="2">
         <v>22297</v>
       </c>
-      <c r="AL3" s="1">
+      <c r="AL3" s="2">
         <v>21996</v>
       </c>
-      <c r="AM3" s="1">
+      <c r="AM3" s="2">
         <v>23089</v>
       </c>
-      <c r="AN3" s="1">
+      <c r="AN3" s="2">
         <v>22866</v>
       </c>
     </row>
-    <row r="4" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1540,44 +1540,44 @@
         <f t="shared" si="72"/>
         <v>734.21373412800017</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AC4" s="2">
         <v>1552</v>
       </c>
-      <c r="AD4" s="1">
+      <c r="AD4" s="2">
         <v>1627</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AE4" s="2">
         <v>1691</v>
       </c>
-      <c r="AF4" s="1">
+      <c r="AF4" s="2">
         <v>1778</v>
       </c>
-      <c r="AG4" s="1">
+      <c r="AG4" s="2">
         <v>1809</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AH4" s="2">
         <v>1879</v>
       </c>
-      <c r="AI4" s="1">
+      <c r="AI4" s="2">
         <v>2051</v>
       </c>
-      <c r="AJ4" s="1">
+      <c r="AJ4" s="2">
         <v>2155</v>
       </c>
-      <c r="AK4" s="1">
+      <c r="AK4" s="2">
         <v>2262</v>
       </c>
-      <c r="AL4" s="1">
+      <c r="AL4" s="2">
         <v>2367</v>
       </c>
-      <c r="AM4" s="1">
+      <c r="AM4" s="2">
         <v>2533</v>
       </c>
-      <c r="AN4" s="1">
+      <c r="AN4" s="2">
         <v>2608</v>
       </c>
     </row>
-    <row r="5" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1638,44 +1638,44 @@
       <c r="U5" s="7">
         <v>0</v>
       </c>
-      <c r="AC5" s="1">
+      <c r="AC5" s="2">
         <v>459</v>
       </c>
-      <c r="AD5" s="1">
+      <c r="AD5" s="2">
         <v>516</v>
       </c>
-      <c r="AE5" s="1">
+      <c r="AE5" s="2">
         <v>561</v>
       </c>
-      <c r="AF5" s="1">
+      <c r="AF5" s="2">
         <v>609</v>
       </c>
-      <c r="AG5" s="1">
+      <c r="AG5" s="2">
         <v>643</v>
       </c>
-      <c r="AH5" s="1">
+      <c r="AH5" s="2">
         <v>692</v>
       </c>
-      <c r="AI5" s="1">
+      <c r="AI5" s="2">
         <v>746</v>
       </c>
-      <c r="AJ5" s="1">
+      <c r="AJ5" s="2">
         <v>698</v>
       </c>
-      <c r="AK5" s="1">
+      <c r="AK5" s="2">
         <v>691</v>
       </c>
-      <c r="AL5" s="1">
+      <c r="AL5" s="2">
         <v>689</v>
       </c>
-      <c r="AM5" s="1">
+      <c r="AM5" s="2">
         <v>614</v>
       </c>
-      <c r="AN5" s="1">
+      <c r="AN5" s="2">
         <v>494</v>
       </c>
     </row>
-    <row r="6" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1740,44 +1740,44 @@
         <f t="shared" si="73"/>
         <v>3.6465187500000007</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AC6" s="2">
         <v>161</v>
       </c>
-      <c r="AD6" s="1">
+      <c r="AD6" s="2">
         <v>-313</v>
       </c>
-      <c r="AE6" s="1">
+      <c r="AE6" s="2">
         <v>150</v>
       </c>
-      <c r="AF6" s="1">
+      <c r="AF6" s="2">
         <v>211</v>
       </c>
-      <c r="AG6" s="1">
+      <c r="AG6" s="2">
         <v>131</v>
       </c>
-      <c r="AH6" s="1">
+      <c r="AH6" s="2">
         <v>71</v>
       </c>
-      <c r="AI6" s="1">
+      <c r="AI6" s="2">
         <v>96</v>
       </c>
-      <c r="AJ6" s="1">
+      <c r="AJ6" s="2">
         <v>87</v>
       </c>
-      <c r="AK6" s="1">
+      <c r="AK6" s="2">
         <v>114</v>
       </c>
-      <c r="AL6" s="1">
+      <c r="AL6" s="2">
         <v>58</v>
       </c>
-      <c r="AM6" s="1">
+      <c r="AM6" s="2">
         <v>-83</v>
       </c>
-      <c r="AN6" s="1">
+      <c r="AN6" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:110" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:110" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5">
-        <f t="shared" ref="Z7:AL7" si="77">SUM(AC3:AC6)</f>
+        <f t="shared" ref="AC7:AK7" si="77">SUM(AC3:AC6)</f>
         <v>24363</v>
       </c>
       <c r="AD7" s="5">
@@ -1909,7 +1909,7 @@
         <v>26013</v>
       </c>
     </row>
-    <row r="8" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1975,44 +1975,44 @@
         <f t="shared" si="79"/>
         <v>1962.0319917228944</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AC8" s="2">
         <v>7704</v>
       </c>
-      <c r="AD8" s="1">
+      <c r="AD8" s="2">
         <v>7680</v>
       </c>
-      <c r="AE8" s="1">
+      <c r="AE8" s="2">
         <v>7937</v>
       </c>
-      <c r="AF8" s="1">
+      <c r="AF8" s="2">
         <v>7206</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AG8" s="2">
         <v>7785</v>
       </c>
-      <c r="AH8" s="1">
+      <c r="AH8" s="2">
         <v>7740</v>
       </c>
-      <c r="AI8" s="1">
+      <c r="AI8" s="2">
         <v>7765</v>
       </c>
-      <c r="AJ8" s="1">
+      <c r="AJ8" s="2">
         <v>7531</v>
       </c>
-      <c r="AK8" s="1">
+      <c r="AK8" s="2">
         <v>7373</v>
       </c>
-      <c r="AL8" s="1">
+      <c r="AL8" s="2">
         <v>7085</v>
       </c>
-      <c r="AM8" s="1">
+      <c r="AM8" s="2">
         <v>7818</v>
       </c>
-      <c r="AN8" s="1">
+      <c r="AN8" s="2">
         <v>7119</v>
       </c>
     </row>
-    <row r="9" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
@@ -2078,44 +2078,44 @@
         <f t="shared" si="80"/>
         <v>1509.2553782483803</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AC9" s="2">
         <v>7471</v>
       </c>
-      <c r="AD9" s="1">
+      <c r="AD9" s="2">
         <v>7181</v>
       </c>
-      <c r="AE9" s="1">
+      <c r="AE9" s="2">
         <v>7118</v>
       </c>
-      <c r="AF9" s="1">
+      <c r="AF9" s="2">
         <v>6803</v>
       </c>
-      <c r="AG9" s="1">
+      <c r="AG9" s="2">
         <v>6577</v>
       </c>
-      <c r="AH9" s="1">
+      <c r="AH9" s="2">
         <v>6580</v>
       </c>
-      <c r="AI9" s="1">
+      <c r="AI9" s="2">
         <v>6407</v>
       </c>
-      <c r="AJ9" s="1">
+      <c r="AJ9" s="2">
         <v>6082</v>
       </c>
-      <c r="AK9" s="1">
+      <c r="AK9" s="2">
         <v>5737</v>
       </c>
-      <c r="AL9" s="1">
+      <c r="AL9" s="2">
         <v>5314</v>
       </c>
-      <c r="AM9" s="1">
+      <c r="AM9" s="2">
         <v>5312</v>
       </c>
-      <c r="AN9" s="1">
+      <c r="AN9" s="2">
         <v>4902</v>
       </c>
     </row>
-    <row r="10" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
@@ -2181,44 +2181,44 @@
         <f t="shared" si="81"/>
         <v>3395.8246010588555</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AC10" s="2">
         <v>9188</v>
       </c>
-      <c r="AD10" s="1">
+      <c r="AD10" s="2">
         <v>8939</v>
       </c>
-      <c r="AE10" s="1">
+      <c r="AE10" s="2">
         <v>9563</v>
       </c>
-      <c r="AF10" s="1">
+      <c r="AF10" s="2">
         <v>10457</v>
       </c>
-      <c r="AG10" s="1">
+      <c r="AG10" s="2">
         <v>10160</v>
       </c>
-      <c r="AH10" s="1">
+      <c r="AH10" s="2">
         <v>11114</v>
       </c>
-      <c r="AI10" s="1">
+      <c r="AI10" s="2">
         <v>11572</v>
       </c>
-      <c r="AJ10" s="1">
+      <c r="AJ10" s="2">
         <v>11963</v>
       </c>
-      <c r="AK10" s="1">
+      <c r="AK10" s="2">
         <v>12254</v>
       </c>
-      <c r="AL10" s="1">
+      <c r="AL10" s="2">
         <v>12711</v>
       </c>
-      <c r="AM10" s="1">
+      <c r="AM10" s="2">
         <v>13023</v>
       </c>
-      <c r="AN10" s="1">
+      <c r="AN10" s="2">
         <v>13992</v>
       </c>
     </row>
-    <row r="11" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2284,44 +2284,44 @@
         <f t="shared" si="82"/>
         <v>679.16492021177112</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AC11" s="2">
         <v>2735</v>
       </c>
-      <c r="AD11" s="1">
+      <c r="AD11" s="2">
         <v>2643</v>
       </c>
-      <c r="AE11" s="1">
+      <c r="AE11" s="2">
         <v>2281</v>
       </c>
-      <c r="AF11" s="1">
+      <c r="AF11" s="2">
         <v>2340</v>
       </c>
-      <c r="AG11" s="1">
+      <c r="AG11" s="2">
         <v>2539</v>
       </c>
-      <c r="AH11" s="1">
+      <c r="AH11" s="2">
         <v>2708</v>
       </c>
-      <c r="AI11" s="1">
+      <c r="AI11" s="2">
         <v>2662</v>
       </c>
-      <c r="AJ11" s="1">
+      <c r="AJ11" s="2">
         <v>2338</v>
       </c>
-      <c r="AK11" s="1">
+      <c r="AK11" s="2">
         <v>2756</v>
       </c>
-      <c r="AL11" s="1">
+      <c r="AL11" s="2">
         <v>2226</v>
       </c>
-      <c r="AM11" s="1">
+      <c r="AM11" s="2">
         <v>2154</v>
       </c>
-      <c r="AN11" s="1">
+      <c r="AN11" s="2">
         <v>2432</v>
       </c>
     </row>
-    <row r="12" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
@@ -2400,44 +2400,44 @@
         <f t="shared" si="85"/>
         <v>3962.8542515625008</v>
       </c>
-      <c r="AC12" s="1">
+      <c r="AC12" s="2">
         <v>6228</v>
       </c>
-      <c r="AD12" s="1">
+      <c r="AD12" s="2">
         <v>6068</v>
       </c>
-      <c r="AE12" s="1">
+      <c r="AE12" s="2">
         <v>7253</v>
       </c>
-      <c r="AF12" s="1">
+      <c r="AF12" s="2">
         <v>8084</v>
       </c>
-      <c r="AG12" s="1">
+      <c r="AG12" s="2">
         <v>7620</v>
       </c>
-      <c r="AH12" s="1">
+      <c r="AH12" s="2">
         <v>8361</v>
       </c>
-      <c r="AI12" s="1">
+      <c r="AI12" s="2">
         <v>8761</v>
       </c>
-      <c r="AJ12" s="1">
+      <c r="AJ12" s="2">
         <v>9593</v>
       </c>
-      <c r="AK12" s="1">
+      <c r="AK12" s="2">
         <v>9115</v>
       </c>
-      <c r="AL12" s="1">
+      <c r="AL12" s="2">
         <v>10326</v>
       </c>
-      <c r="AM12" s="1">
+      <c r="AM12" s="2">
         <v>10873</v>
       </c>
-      <c r="AN12" s="1">
+      <c r="AN12" s="2">
         <v>11560</v>
       </c>
     </row>
-    <row r="13" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
@@ -2487,44 +2487,44 @@
       <c r="Q13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
-      <c r="AC13" s="1">
+      <c r="AC13" s="2">
         <v>1133</v>
       </c>
-      <c r="AD13" s="1">
+      <c r="AD13" s="2">
         <v>1216</v>
       </c>
-      <c r="AE13" s="1">
+      <c r="AE13" s="2">
         <v>1126</v>
       </c>
-      <c r="AF13" s="1">
+      <c r="AF13" s="2">
         <v>1049</v>
       </c>
-      <c r="AG13" s="1">
+      <c r="AG13" s="2">
         <v>808</v>
       </c>
-      <c r="AH13" s="1">
+      <c r="AH13" s="2">
         <v>817</v>
       </c>
-      <c r="AI13" s="1">
+      <c r="AI13" s="2">
         <v>747</v>
       </c>
-      <c r="AJ13" s="1">
+      <c r="AJ13" s="2">
         <v>705</v>
       </c>
-      <c r="AK13" s="1">
+      <c r="AK13" s="2">
         <v>665</v>
       </c>
-      <c r="AL13" s="1">
+      <c r="AL13" s="2">
         <v>1280</v>
       </c>
-      <c r="AM13" s="1">
+      <c r="AM13" s="2">
         <v>1209</v>
       </c>
-      <c r="AN13" s="1">
+      <c r="AN13" s="2">
         <v>1162</v>
       </c>
     </row>
-    <row r="14" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
@@ -2573,44 +2573,44 @@
       <c r="Q14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
-      <c r="AC14" s="1">
+      <c r="AC14" s="2">
         <v>5723</v>
       </c>
-      <c r="AD14" s="1">
+      <c r="AD14" s="2">
         <v>5582</v>
       </c>
-      <c r="AE14" s="1">
+      <c r="AE14" s="2">
         <v>6477</v>
       </c>
-      <c r="AF14" s="1">
+      <c r="AF14" s="2">
         <v>6942</v>
       </c>
-      <c r="AG14" s="1">
+      <c r="AG14" s="2">
         <v>7774</v>
       </c>
-      <c r="AH14" s="1">
+      <c r="AH14" s="2">
         <v>8078</v>
       </c>
-      <c r="AI14" s="1">
+      <c r="AI14" s="2">
         <v>21852</v>
       </c>
-      <c r="AJ14" s="1">
+      <c r="AJ14" s="2">
         <v>9828</v>
       </c>
-      <c r="AK14" s="1">
+      <c r="AK14" s="2">
         <v>9341</v>
       </c>
-      <c r="AL14" s="1">
+      <c r="AL14" s="2">
         <v>766</v>
       </c>
-      <c r="AM14" s="1">
+      <c r="AM14" s="2">
         <v>6890</v>
       </c>
-      <c r="AN14" s="1">
+      <c r="AN14" s="2">
         <v>3842</v>
       </c>
     </row>
-    <row r="15" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:110" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
@@ -2694,7 +2694,7 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2">
-        <f t="shared" ref="Z15:AL15" si="88">AC14-AC16</f>
+        <f t="shared" ref="AC15:AK15" si="88">AC14-AC16</f>
         <v>1818</v>
       </c>
       <c r="AD15" s="2">
@@ -2742,7 +2742,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="16" spans="1:110" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:110" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
@@ -2808,40 +2808,40 @@
         <f t="shared" si="90"/>
         <v>1962.0319917228944</v>
       </c>
-      <c r="AC16" s="4">
+      <c r="AC16" s="5">
         <v>3905</v>
       </c>
-      <c r="AD16" s="4">
+      <c r="AD16" s="5">
         <v>3390</v>
       </c>
-      <c r="AE16" s="4">
+      <c r="AE16" s="5">
         <v>4183</v>
       </c>
-      <c r="AF16" s="4">
+      <c r="AF16" s="5">
         <v>4535</v>
       </c>
-      <c r="AG16" s="4">
+      <c r="AG16" s="5">
         <v>5070</v>
       </c>
-      <c r="AH16" s="4">
+      <c r="AH16" s="5">
         <v>5243</v>
       </c>
-      <c r="AI16" s="4">
+      <c r="AI16" s="5">
         <v>14239</v>
       </c>
-      <c r="AJ16" s="4">
+      <c r="AJ16" s="5">
         <v>10222</v>
       </c>
-      <c r="AK16" s="4">
+      <c r="AK16" s="5">
         <v>6963</v>
       </c>
-      <c r="AL16" s="4">
+      <c r="AL16" s="5">
         <v>-1298</v>
       </c>
-      <c r="AM16" s="4">
+      <c r="AM16" s="5">
         <v>4467</v>
       </c>
-      <c r="AN16" s="4">
+      <c r="AN16" s="5">
         <v>2475</v>
       </c>
       <c r="AO16" s="5">
@@ -3125,7 +3125,7 @@
         <v>1.6556306886972949E-15</v>
       </c>
     </row>
-    <row r="17" spans="2:43" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="18" spans="2:43" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
     </row>
-    <row r="20" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>50</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>-5.6660899653979246E-2</v>
       </c>
       <c r="AD20" s="9">
-        <f t="shared" ref="AD20:AJ20" si="97">AD7/AC7-1</f>
+        <f t="shared" ref="AD20:AI20" si="97">AD7/AC7-1</f>
         <v>-2.310881254361119E-2</v>
       </c>
       <c r="AE20" s="9">
@@ -3406,7 +3406,7 @@
         <v>-5.3531143654648172E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>51</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>0.15191808039125784</v>
       </c>
       <c r="AC21" s="9">
-        <f t="shared" ref="AC21:AJ21" si="100">AC15/AC14</f>
+        <f t="shared" ref="AC21:AI21" si="100">AC15/AC14</f>
         <v>0.31766556002096802</v>
       </c>
       <c r="AD21" s="9">
@@ -3495,7 +3495,7 @@
         <v>0.34838916346329857</v>
       </c>
       <c r="AJ21" s="9">
-        <f t="shared" ref="AI21:AN21" si="101">AJ15/AJ14</f>
+        <f t="shared" ref="AJ21:AM21" si="101">AJ15/AJ14</f>
         <v>-4.0089540089540091E-2</v>
       </c>
       <c r="AK21" s="9">
@@ -3515,7 +3515,7 @@
         <v>0.35580426861009889</v>
       </c>
     </row>
-    <row r="22" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>52</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>0.53788490370199515</v>
       </c>
     </row>
-    <row r="23" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>53</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>0.2610423353201895</v>
       </c>
     </row>
-    <row r="24" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>54</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>8.5740486015589173E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>32</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>55</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="27" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>56</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>2592.8571428571422</v>
       </c>
     </row>
-    <row r="28" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>57</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>58.635394456289966</v>
       </c>
     </row>
-    <row r="29" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>58</v>
       </c>
@@ -4101,7 +4101,7 @@
       <c r="AP29" s="22"/>
       <c r="AQ29" s="25"/>
     </row>
-    <row r="30" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:43" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
       <c r="Q30" s="11"/>
       <c r="R30" s="12"/>
@@ -4110,7 +4110,7 @@
         <v>59</v>
       </c>
       <c r="AD30" s="9">
-        <f t="shared" ref="AD30:AN30" si="113">AD16/AC16-1</f>
+        <f t="shared" ref="AD30:AM30" si="113">AD16/AC16-1</f>
         <v>-0.13188220230473746</v>
       </c>
       <c r="AE30" s="9">
@@ -4161,12 +4161,12 @@
         <v>0.32599263808887313</v>
       </c>
     </row>
-    <row r="31" spans="2:43" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:43" x14ac:dyDescent="0.25">
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
       <c r="S31" s="13"/>
     </row>
-    <row r="32" spans="2:43" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>36</v>
       </c>
@@ -4229,7 +4229,7 @@
       <c r="AP32" s="27"/>
       <c r="AQ32" s="27"/>
     </row>
-    <row r="33" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>41</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>42</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="36" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>4345</v>
       </c>
     </row>
-    <row r="37" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>376746</v>
       </c>
     </row>
-    <row r="38" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="39" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>25046</v>
       </c>
     </row>
-    <row r="40" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>43</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>39149</v>
       </c>
     </row>
-    <row r="41" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>39</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>2403</v>
       </c>
     </row>
-    <row r="42" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>44</v>
       </c>

</xml_diff>